<commit_message>
v0.23 - Open Operation
</commit_message>
<xml_diff>
--- a/static/paper/APD05_paper.xlsx
+++ b/static/paper/APD05_paper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\paper_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\SnowBall\static\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD06071D-3ED4-4947-901B-1F5DCC175A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA582BC5-3908-4B3B-929B-2276158031BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5E3EE22-C542-4402-8654-7D4EE4676255}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5E3EE22-C542-4402-8654-7D4EE4676255}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing Table" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Prior year control testing documentation rolled forward for reference purposes.</t>
   </si>
@@ -139,11 +139,23 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>최소자리</t>
+    <t>관리자ID</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>복잡성</t>
+    <t>사용자명</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>부서명</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>직무</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>권한 보유 적정성 검토</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -249,12 +261,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="바탕"/>
-      <family val="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +304,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -556,7 +575,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -922,45 +941,52 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G8"/>
+  <dimension ref="B1:J8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="5" style="2" customWidth="1"/>
-    <col min="3" max="4" width="15.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2"/>
-    <col min="9" max="9" width="9.140625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="6" width="15.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="2"/>
+    <col min="12" max="12" width="9.140625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" s="1" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
     </row>
-    <row r="2" spans="2:7" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
     </row>
-    <row r="4" spans="2:7" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" s="3" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
@@ -970,32 +996,47 @@
       <c r="D4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="I4" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>1</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:7" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>5</v>
       </c>
@@ -1003,8 +1044,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>